<commit_message>
modified tutorials, added example data
Tutorial codes are modified due to changes made to stoichiometry calculation and ternary plots.
More example data are added to the input xlsx files (in "Sheet2") for comparison with results calculated from the excel version of pyAp (ApThermo).
</commit_message>
<xml_diff>
--- a/tutorial/data_ap_major_volatile.xlsx
+++ b/tutorial/data_ap_major_volatile.xlsx
@@ -1,20 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexweiranli/Documents/0python/pyAp-main/example/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8DCCB5-DA6F-4749-BD02-C6B6D2E44B95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="840" yWindow="500" windowWidth="25260" windowHeight="16520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
   <si>
     <t>sample</t>
   </si>
@@ -73,9 +92,6 @@
     <t>TOTAL</t>
   </si>
   <si>
-    <t>OXYGEN NUMBER</t>
-  </si>
-  <si>
     <t>Ap1</t>
   </si>
   <si>
@@ -83,13 +99,25 @@
   </si>
   <si>
     <t>Ap3</t>
+  </si>
+  <si>
+    <t>Ap1c</t>
+  </si>
+  <si>
+    <t>Ap2c</t>
+  </si>
+  <si>
+    <t>Ap3c</t>
+  </si>
+  <si>
+    <t>Ap4c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,8 +126,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -141,10 +176,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -152,6 +196,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -198,7 +250,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -230,9 +282,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -264,6 +334,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -439,14 +527,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="8.83203125" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -504,186 +597,439 @@
       <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="B2" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F2" s="2">
+        <v>54</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="M2" s="2">
+        <v>40</v>
+      </c>
+      <c r="N2" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="O2" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="P2" s="2">
+        <v>3</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="S2" s="2">
+        <v>98.810000000000016</v>
+      </c>
     </row>
-    <row r="2" spans="1:20">
-      <c r="A2" t="s">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B2">
-        <v>0.1</v>
-      </c>
-      <c r="C2">
-        <v>0.1</v>
-      </c>
-      <c r="D2">
-        <v>0.1</v>
-      </c>
-      <c r="E2">
-        <v>0.1</v>
-      </c>
-      <c r="F2">
+      <c r="B3" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F3" s="2">
         <v>54</v>
       </c>
-      <c r="G2">
-        <v>0.1</v>
-      </c>
-      <c r="H2">
-        <v>0.1</v>
-      </c>
-      <c r="I2">
-        <v>0.1</v>
-      </c>
-      <c r="J2">
-        <v>0.1</v>
-      </c>
-      <c r="K2">
+      <c r="G3" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="K3" s="2">
         <v>0.2</v>
       </c>
-      <c r="L2">
-        <v>0.1</v>
-      </c>
-      <c r="M2">
+      <c r="L3" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="M3" s="2">
         <v>40</v>
       </c>
-      <c r="N2">
+      <c r="N3" s="2">
         <v>0.2</v>
       </c>
-      <c r="O2">
+      <c r="O3" s="2">
         <v>0.01</v>
       </c>
-      <c r="P2">
+      <c r="P3" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="S3" s="2">
+        <v>98.210000000000022</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F4" s="2">
+        <v>54</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="M4" s="2">
+        <v>40</v>
+      </c>
+      <c r="N4" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="O4" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="P4" s="2">
+        <v>2.8</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="S4" s="2">
+        <v>98.910000000000011</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED85638-A4C6-3046-ACEA-35A140AE6303}">
+  <dimension ref="A1:S5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="Q2">
-        <v>0.5</v>
-      </c>
-      <c r="S2">
-        <v>98.81000000000002</v>
-      </c>
-      <c r="T2">
-        <v>25.89795036358714</v>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
-      <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3">
-        <v>0.1</v>
-      </c>
-      <c r="C3">
-        <v>0.1</v>
-      </c>
-      <c r="D3">
-        <v>0.1</v>
-      </c>
-      <c r="E3">
-        <v>0.1</v>
-      </c>
-      <c r="F3">
-        <v>54</v>
-      </c>
-      <c r="G3">
-        <v>0.1</v>
-      </c>
-      <c r="H3">
-        <v>0.1</v>
-      </c>
-      <c r="I3">
-        <v>0.1</v>
-      </c>
-      <c r="J3">
-        <v>0.1</v>
-      </c>
-      <c r="K3">
+    <row r="2" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2">
+        <v>0.32</v>
+      </c>
+      <c r="F2" s="2">
+        <v>54.12</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="H2" s="2">
         <v>0.2</v>
       </c>
-      <c r="L3">
-        <v>0.1</v>
-      </c>
-      <c r="M3">
-        <v>40</v>
-      </c>
-      <c r="N3">
+      <c r="I2" s="2"/>
+      <c r="J2" s="2">
+        <v>0.11</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="M2" s="2">
+        <v>41.28</v>
+      </c>
+      <c r="N2" s="2">
+        <v>0.13</v>
+      </c>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2">
+        <v>1.46</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>1.17</v>
+      </c>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+    </row>
+    <row r="3" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.26</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2">
+        <v>0.32</v>
+      </c>
+      <c r="F3" s="2">
+        <v>53.68</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.33</v>
+      </c>
+      <c r="H3" s="2">
         <v>0.2</v>
       </c>
-      <c r="O3">
-        <v>0.01</v>
-      </c>
-      <c r="P3">
+      <c r="I3" s="2"/>
+      <c r="J3" s="2">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="M3" s="2">
+        <v>41.16</v>
+      </c>
+      <c r="N3" s="2">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2">
         <v>2.5</v>
       </c>
-      <c r="Q3">
-        <v>0.4</v>
-      </c>
-      <c r="S3">
-        <v>98.21000000000002</v>
-      </c>
-      <c r="T3">
-        <v>25.74806911091732</v>
-      </c>
+      <c r="Q3" s="2">
+        <v>0.89</v>
+      </c>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
     </row>
-    <row r="4" spans="1:20">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4">
-        <v>0.1</v>
-      </c>
-      <c r="C4">
-        <v>0.1</v>
-      </c>
-      <c r="D4">
-        <v>0.1</v>
-      </c>
-      <c r="E4">
-        <v>0.1</v>
-      </c>
-      <c r="F4">
-        <v>54</v>
-      </c>
-      <c r="G4">
-        <v>0.1</v>
-      </c>
-      <c r="H4">
-        <v>0.1</v>
-      </c>
-      <c r="I4">
-        <v>0.1</v>
-      </c>
-      <c r="J4">
-        <v>0.1</v>
-      </c>
-      <c r="K4">
+    <row r="4" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.19719500000000001</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2">
+        <v>0.32</v>
+      </c>
+      <c r="F4" s="2">
+        <v>53.8</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.345082</v>
+      </c>
+      <c r="H4" s="2">
         <v>0.2</v>
       </c>
-      <c r="L4">
-        <v>0.1</v>
-      </c>
-      <c r="M4">
-        <v>40</v>
-      </c>
-      <c r="N4">
+      <c r="I4" s="2"/>
+      <c r="J4" s="2">
+        <v>7.8275999999999998E-2</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0.187502</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="M4" s="2">
+        <v>40.963700000000003</v>
+      </c>
+      <c r="N4" s="2">
+        <v>7.5556999999999999E-2</v>
+      </c>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2">
+        <v>2.50149</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>0.85453400000000002</v>
+      </c>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+    </row>
+    <row r="5" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.26232299999999997</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2">
+        <v>0.32</v>
+      </c>
+      <c r="F5" s="2">
+        <v>53.506700000000002</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.34916999999999998</v>
+      </c>
+      <c r="H5" s="2">
         <v>0.2</v>
       </c>
-      <c r="O4">
-        <v>0.01</v>
-      </c>
-      <c r="P4">
-        <v>2.8</v>
-      </c>
-      <c r="Q4">
-        <v>0.8</v>
-      </c>
-      <c r="S4">
-        <v>98.91000000000001</v>
-      </c>
-      <c r="T4">
-        <v>25.8873555573784</v>
-      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2">
+        <v>7.3810000000000001E-2</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0.241928</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="M5" s="2">
+        <v>41.081899999999997</v>
+      </c>
+      <c r="N5" s="2">
+        <v>0.112334</v>
+      </c>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2">
+        <v>2.0448900000000001</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>0.95819200000000004</v>
+      </c>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>